<commit_message>
Updated Data files and country stats files
</commit_message>
<xml_diff>
--- a/source_data/RAPP_2013.xlsx
+++ b/source_data/RAPP_2013.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25915"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="8000" yWindow="520" windowWidth="20540" windowHeight="11480" tabRatio="485"/>
+    <workbookView xWindow="8000" yWindow="520" windowWidth="20540" windowHeight="11480" tabRatio="485" firstSheet="2" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Complete List TDA TVRPA EO" sheetId="1" r:id="rId1"/>
@@ -1629,7 +1629,7 @@
     <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
-  <fonts count="17" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1735,6 +1735,28 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial Narrow"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Arial Narrow"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="13">
@@ -1916,7 +1938,7 @@
     <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="164" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="99">
+  <cellXfs count="103">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -2185,6 +2207,18 @@
     </xf>
     <xf numFmtId="49" fontId="12" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -2492,7 +2526,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B153"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A132" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
@@ -3743,7 +3777,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B139"/>
   <sheetViews>
-    <sheetView topLeftCell="A49" workbookViewId="0">
+    <sheetView topLeftCell="A63" workbookViewId="0">
       <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
@@ -4879,7 +4913,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E354"/>
   <sheetViews>
-    <sheetView topLeftCell="A325" workbookViewId="0">
+    <sheetView topLeftCell="A36" workbookViewId="0">
       <selection activeCell="A358" sqref="A358"/>
     </sheetView>
   </sheetViews>
@@ -9761,8 +9795,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S159"/>
   <sheetViews>
-    <sheetView topLeftCell="A94" workbookViewId="0">
-      <selection activeCell="A43" sqref="A43"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -9902,7 +9936,9 @@
       <c r="C4" s="43"/>
       <c r="D4" s="43"/>
       <c r="E4" s="44"/>
-      <c r="F4" s="44"/>
+      <c r="F4" s="101">
+        <v>673949</v>
+      </c>
       <c r="G4" s="45"/>
       <c r="H4" s="46"/>
       <c r="I4" s="43"/>
@@ -9933,7 +9969,9 @@
       <c r="E5" s="44" t="s">
         <v>408</v>
       </c>
-      <c r="F5" s="44"/>
+      <c r="F5" s="102">
+        <v>23665</v>
+      </c>
       <c r="G5" s="45">
         <v>4.5686204717211751</v>
       </c>
@@ -9978,7 +10016,7 @@
       <c r="C6" s="43"/>
       <c r="D6" s="43"/>
       <c r="E6" s="44"/>
-      <c r="F6" s="44"/>
+      <c r="F6" s="100"/>
       <c r="G6" s="45"/>
       <c r="H6" s="46"/>
       <c r="I6" s="43"/>
@@ -10013,7 +10051,7 @@
       <c r="E7" s="44" t="s">
         <v>408</v>
       </c>
-      <c r="F7" s="44"/>
+      <c r="F7" s="100"/>
       <c r="G7" s="45">
         <v>25.7</v>
       </c>
@@ -10056,7 +10094,7 @@
       <c r="C8" s="43"/>
       <c r="D8" s="43"/>
       <c r="E8" s="44"/>
-      <c r="F8" s="44"/>
+      <c r="F8" s="100"/>
       <c r="G8" s="45"/>
       <c r="H8" s="46"/>
       <c r="I8" s="43"/>
@@ -10087,7 +10125,7 @@
       <c r="E9" s="44" t="s">
         <v>408</v>
       </c>
-      <c r="F9" s="44"/>
+      <c r="F9" s="99"/>
       <c r="G9" s="45">
         <v>11</v>
       </c>
@@ -10144,7 +10182,7 @@
       <c r="E10" s="44" t="s">
         <v>408</v>
       </c>
-      <c r="F10" s="44"/>
+      <c r="F10" s="100"/>
       <c r="G10" s="45">
         <v>8.1</v>
       </c>
@@ -10195,7 +10233,7 @@
       <c r="E11" s="44" t="s">
         <v>408</v>
       </c>
-      <c r="F11" s="44"/>
+      <c r="F11" s="100"/>
       <c r="G11" s="45">
         <v>4.5</v>
       </c>
@@ -10244,7 +10282,7 @@
       <c r="C12" s="43"/>
       <c r="D12" s="43"/>
       <c r="E12" s="44"/>
-      <c r="F12" s="44"/>
+      <c r="F12" s="100"/>
       <c r="G12" s="45"/>
       <c r="H12" s="46"/>
       <c r="I12" s="43"/>
@@ -10275,7 +10313,7 @@
       <c r="E13" s="53" t="s">
         <v>408</v>
       </c>
-      <c r="F13" s="53"/>
+      <c r="F13" s="100"/>
       <c r="G13" s="54">
         <v>10.1</v>
       </c>
@@ -10324,7 +10362,7 @@
       <c r="C14" s="43"/>
       <c r="D14" s="43"/>
       <c r="E14" s="44"/>
-      <c r="F14" s="44"/>
+      <c r="F14" s="100"/>
       <c r="G14" s="45"/>
       <c r="H14" s="46"/>
       <c r="I14" s="43"/>
@@ -10359,7 +10397,7 @@
       <c r="E15" s="44" t="s">
         <v>408</v>
       </c>
-      <c r="F15" s="44"/>
+      <c r="F15" s="99"/>
       <c r="G15" s="45">
         <v>8.3000000000000007</v>
       </c>
@@ -10410,7 +10448,7 @@
       <c r="E16" s="43" t="s">
         <v>408</v>
       </c>
-      <c r="F16" s="43"/>
+      <c r="F16" s="100"/>
       <c r="G16" s="45">
         <v>31.5</v>
       </c>
@@ -10461,7 +10499,7 @@
       <c r="E17" s="44" t="s">
         <v>408</v>
       </c>
-      <c r="F17" s="44"/>
+      <c r="F17" s="99"/>
       <c r="G17" s="45">
         <v>3.8</v>
       </c>
@@ -10512,7 +10550,7 @@
       <c r="E18" s="44" t="s">
         <v>409</v>
       </c>
-      <c r="F18" s="44"/>
+      <c r="F18" s="100"/>
       <c r="G18" s="45">
         <v>20.2</v>
       </c>
@@ -10569,7 +10607,7 @@
       <c r="E19" s="44" t="s">
         <v>408</v>
       </c>
-      <c r="F19" s="44"/>
+      <c r="F19" s="100"/>
       <c r="G19" s="45">
         <v>8.9</v>
       </c>
@@ -10608,7 +10646,7 @@
       <c r="C20" s="43"/>
       <c r="D20" s="43"/>
       <c r="E20" s="44"/>
-      <c r="F20" s="44"/>
+      <c r="F20" s="100"/>
       <c r="G20" s="45"/>
       <c r="H20" s="46"/>
       <c r="I20" s="43"/>
@@ -10643,7 +10681,7 @@
       <c r="E21" s="44" t="s">
         <v>408</v>
       </c>
-      <c r="F21" s="44"/>
+      <c r="F21" s="100"/>
       <c r="G21" s="45">
         <v>3.4751168802840926</v>
       </c>
@@ -10688,7 +10726,7 @@
       <c r="C22" s="43"/>
       <c r="D22" s="43"/>
       <c r="E22" s="44"/>
-      <c r="F22" s="44"/>
+      <c r="F22" s="100"/>
       <c r="G22" s="45"/>
       <c r="H22" s="46"/>
       <c r="I22" s="45"/>
@@ -10711,7 +10749,7 @@
       <c r="C23" s="43"/>
       <c r="D23" s="43"/>
       <c r="E23" s="44"/>
-      <c r="F23" s="44"/>
+      <c r="F23" s="100"/>
       <c r="G23" s="45"/>
       <c r="H23" s="46"/>
       <c r="I23" s="45"/>
@@ -10746,7 +10784,7 @@
       <c r="E24" s="44" t="s">
         <v>408</v>
       </c>
-      <c r="F24" s="44"/>
+      <c r="F24" s="100"/>
       <c r="G24" s="45">
         <v>42.1</v>
       </c>
@@ -10797,7 +10835,7 @@
       <c r="E25" s="44" t="s">
         <v>408</v>
       </c>
-      <c r="F25" s="44"/>
+      <c r="F25" s="100"/>
       <c r="G25" s="45">
         <v>27.17</v>
       </c>
@@ -10848,7 +10886,7 @@
       <c r="E26" s="44" t="s">
         <v>436</v>
       </c>
-      <c r="F26" s="44"/>
+      <c r="F26" s="100"/>
       <c r="G26" s="45">
         <v>3.2</v>
       </c>
@@ -10905,7 +10943,7 @@
       <c r="E27" s="44" t="s">
         <v>408</v>
       </c>
-      <c r="F27" s="44"/>
+      <c r="F27" s="99"/>
       <c r="G27" s="45">
         <v>28.65</v>
       </c>
@@ -10962,7 +11000,7 @@
       <c r="E28" s="44" t="s">
         <v>408</v>
       </c>
-      <c r="F28" s="44"/>
+      <c r="F28" s="59"/>
       <c r="G28" s="45">
         <v>56.2</v>
       </c>
@@ -11011,7 +11049,7 @@
       <c r="E29" s="44" t="s">
         <v>408</v>
       </c>
-      <c r="F29" s="44"/>
+      <c r="F29" s="100"/>
       <c r="G29" s="45">
         <v>51.1</v>
       </c>
@@ -11062,7 +11100,7 @@
       <c r="E30" s="44" t="s">
         <v>408</v>
       </c>
-      <c r="F30" s="44"/>
+      <c r="F30" s="99"/>
       <c r="G30" s="45">
         <v>53</v>
       </c>
@@ -11113,7 +11151,7 @@
       <c r="E31" s="44" t="s">
         <v>408</v>
       </c>
-      <c r="F31" s="44"/>
+      <c r="F31" s="99"/>
       <c r="G31" s="45">
         <v>3.5</v>
       </c>
@@ -11162,7 +11200,7 @@
       <c r="C32" s="43"/>
       <c r="D32" s="43"/>
       <c r="E32" s="44"/>
-      <c r="F32" s="44"/>
+      <c r="F32" s="99"/>
       <c r="G32" s="45"/>
       <c r="H32" s="46"/>
       <c r="I32" s="43"/>
@@ -11185,7 +11223,7 @@
       <c r="C33" s="43"/>
       <c r="D33" s="43"/>
       <c r="E33" s="44"/>
-      <c r="F33" s="44"/>
+      <c r="F33" s="100"/>
       <c r="G33" s="45"/>
       <c r="H33" s="46"/>
       <c r="I33" s="43"/>
@@ -11216,7 +11254,7 @@
       <c r="E34" s="53" t="s">
         <v>408</v>
       </c>
-      <c r="F34" s="53"/>
+      <c r="F34" s="100"/>
       <c r="G34" s="54">
         <v>5.9284256415702981</v>
       </c>
@@ -11273,7 +11311,7 @@
       <c r="E35" s="44" t="s">
         <v>408</v>
       </c>
-      <c r="F35" s="44"/>
+      <c r="F35" s="100"/>
       <c r="G35" s="45">
         <v>35.6</v>
       </c>
@@ -11324,7 +11362,7 @@
       <c r="E36" s="44" t="s">
         <v>408</v>
       </c>
-      <c r="F36" s="44"/>
+      <c r="F36" s="99"/>
       <c r="G36" s="45">
         <v>16.933738872541269</v>
       </c>
@@ -11375,7 +11413,7 @@
       <c r="E37" s="44" t="s">
         <v>408</v>
       </c>
-      <c r="F37" s="44"/>
+      <c r="F37" s="99"/>
       <c r="G37" s="45">
         <v>27</v>
       </c>
@@ -11418,7 +11456,7 @@
       <c r="C38" s="43"/>
       <c r="D38" s="43"/>
       <c r="E38" s="44"/>
-      <c r="F38" s="44"/>
+      <c r="F38" s="100"/>
       <c r="G38" s="45"/>
       <c r="H38" s="46"/>
       <c r="I38" s="43"/>
@@ -11453,7 +11491,7 @@
       <c r="E39" s="44" t="s">
         <v>408</v>
       </c>
-      <c r="F39" s="44"/>
+      <c r="F39" s="100"/>
       <c r="G39" s="45">
         <v>2.1697274682663932</v>
       </c>
@@ -11510,7 +11548,7 @@
       <c r="E40" s="44" t="s">
         <v>408</v>
       </c>
-      <c r="F40" s="44"/>
+      <c r="F40" s="99"/>
       <c r="G40" s="45">
         <v>39.799999999999997</v>
       </c>
@@ -11561,7 +11599,7 @@
       <c r="E41" s="44" t="s">
         <v>408</v>
       </c>
-      <c r="F41" s="44"/>
+      <c r="F41" s="99"/>
       <c r="G41" s="45">
         <v>12.3</v>
       </c>
@@ -11604,7 +11642,7 @@
       <c r="C42" s="43"/>
       <c r="D42" s="43"/>
       <c r="E42" s="44"/>
-      <c r="F42" s="44"/>
+      <c r="F42" s="100"/>
       <c r="G42" s="45"/>
       <c r="H42" s="46"/>
       <c r="I42" s="43"/>
@@ -11639,7 +11677,7 @@
       <c r="E43" s="44" t="s">
         <v>436</v>
       </c>
-      <c r="F43" s="44"/>
+      <c r="F43" s="100"/>
       <c r="G43" s="45">
         <v>5.3</v>
       </c>
@@ -11696,7 +11734,7 @@
       <c r="E44" s="53" t="s">
         <v>408</v>
       </c>
-      <c r="F44" s="53"/>
+      <c r="F44" s="100"/>
       <c r="G44" s="54">
         <v>2.7229398341599915</v>
       </c>
@@ -11753,7 +11791,7 @@
       <c r="E45" s="44" t="s">
         <v>408</v>
       </c>
-      <c r="F45" s="44"/>
+      <c r="F45" s="100"/>
       <c r="G45" s="45">
         <v>6.7</v>
       </c>
@@ -11804,7 +11842,7 @@
       <c r="E46" s="44" t="s">
         <v>408</v>
       </c>
-      <c r="F46" s="44"/>
+      <c r="F46" s="100"/>
       <c r="G46" s="45">
         <v>6.3</v>
       </c>
@@ -11853,7 +11891,7 @@
       <c r="C47" s="58"/>
       <c r="D47" s="58"/>
       <c r="E47" s="59"/>
-      <c r="F47" s="59"/>
+      <c r="F47" s="100"/>
       <c r="G47" s="60"/>
       <c r="H47" s="61"/>
       <c r="I47" s="58"/>
@@ -11888,7 +11926,7 @@
       <c r="E48" s="59" t="s">
         <v>408</v>
       </c>
-      <c r="F48" s="59"/>
+      <c r="F48" s="100"/>
       <c r="G48" s="60">
         <v>22</v>
       </c>
@@ -11931,7 +11969,7 @@
       <c r="C49" s="58"/>
       <c r="D49" s="58"/>
       <c r="E49" s="59"/>
-      <c r="F49" s="59"/>
+      <c r="F49" s="100"/>
       <c r="G49" s="60"/>
       <c r="H49" s="61"/>
       <c r="I49" s="58"/>
@@ -11954,7 +11992,7 @@
       <c r="C50" s="58"/>
       <c r="D50" s="58"/>
       <c r="E50" s="59"/>
-      <c r="F50" s="59"/>
+      <c r="F50" s="100"/>
       <c r="G50" s="60"/>
       <c r="H50" s="61"/>
       <c r="I50" s="58"/>
@@ -11981,7 +12019,7 @@
       <c r="C51" s="58"/>
       <c r="D51" s="58"/>
       <c r="E51" s="59"/>
-      <c r="F51" s="59"/>
+      <c r="F51" s="100"/>
       <c r="G51" s="60"/>
       <c r="H51" s="61"/>
       <c r="I51" s="58"/>
@@ -12012,7 +12050,7 @@
       <c r="E52" s="44" t="s">
         <v>408</v>
       </c>
-      <c r="F52" s="44"/>
+      <c r="F52" s="100"/>
       <c r="G52" s="45">
         <v>36.4</v>
       </c>
@@ -12063,7 +12101,7 @@
       <c r="E53" s="44" t="s">
         <v>408</v>
       </c>
-      <c r="F53" s="44"/>
+      <c r="F53" s="100"/>
       <c r="G53" s="45">
         <v>29.1</v>
       </c>
@@ -12114,7 +12152,7 @@
       <c r="E54" s="44" t="s">
         <v>408</v>
       </c>
-      <c r="F54" s="44"/>
+      <c r="F54" s="100"/>
       <c r="G54" s="45">
         <v>43.5</v>
       </c>
@@ -12157,7 +12195,7 @@
       <c r="C55" s="43"/>
       <c r="D55" s="43"/>
       <c r="E55" s="44"/>
-      <c r="F55" s="44"/>
+      <c r="F55" s="99"/>
       <c r="G55" s="45"/>
       <c r="H55" s="46"/>
       <c r="I55" s="43"/>
@@ -12180,7 +12218,7 @@
       <c r="C56" s="43"/>
       <c r="D56" s="43"/>
       <c r="E56" s="44"/>
-      <c r="F56" s="44"/>
+      <c r="F56" s="100"/>
       <c r="G56" s="45"/>
       <c r="H56" s="46"/>
       <c r="I56" s="43"/>
@@ -12215,7 +12253,7 @@
       <c r="E57" s="44" t="s">
         <v>409</v>
       </c>
-      <c r="F57" s="44"/>
+      <c r="F57" s="100"/>
       <c r="G57" s="45">
         <v>13.4</v>
       </c>
@@ -12272,7 +12310,7 @@
       <c r="E58" s="44" t="s">
         <v>408</v>
       </c>
-      <c r="F58" s="44"/>
+      <c r="F58" s="100"/>
       <c r="G58" s="45">
         <v>38.797051682275409</v>
       </c>
@@ -12329,7 +12367,7 @@
       <c r="E59" s="44" t="s">
         <v>408</v>
       </c>
-      <c r="F59" s="44"/>
+      <c r="F59" s="100"/>
       <c r="G59" s="45">
         <v>47.3</v>
       </c>
@@ -12380,7 +12418,7 @@
       <c r="E60" s="44" t="s">
         <v>408</v>
       </c>
-      <c r="F60" s="44"/>
+      <c r="F60" s="100"/>
       <c r="G60" s="45">
         <v>23</v>
       </c>
@@ -12431,7 +12469,7 @@
       <c r="E61" s="44" t="s">
         <v>408</v>
       </c>
-      <c r="F61" s="44"/>
+      <c r="F61" s="99"/>
       <c r="G61" s="45">
         <v>29</v>
       </c>
@@ -12470,7 +12508,7 @@
       <c r="C62" s="43"/>
       <c r="D62" s="43"/>
       <c r="E62" s="44"/>
-      <c r="F62" s="44"/>
+      <c r="F62" s="99"/>
       <c r="G62" s="45"/>
       <c r="H62" s="46"/>
       <c r="I62" s="43"/>
@@ -12501,7 +12539,7 @@
       <c r="E63" s="43" t="s">
         <v>408</v>
       </c>
-      <c r="F63" s="43"/>
+      <c r="F63" s="100"/>
       <c r="G63" s="43">
         <v>7.2</v>
       </c>
@@ -12558,7 +12596,7 @@
       <c r="E64" s="44" t="s">
         <v>408</v>
       </c>
-      <c r="F64" s="44"/>
+      <c r="F64" s="100"/>
       <c r="G64" s="45">
         <v>1.97</v>
       </c>
@@ -12615,7 +12653,7 @@
       <c r="E65" s="44" t="s">
         <v>436</v>
       </c>
-      <c r="F65" s="44"/>
+      <c r="F65" s="99"/>
       <c r="G65" s="45">
         <v>3.7</v>
       </c>
@@ -12672,7 +12710,7 @@
       <c r="E66" s="44" t="s">
         <v>408</v>
       </c>
-      <c r="F66" s="44"/>
+      <c r="F66" s="100"/>
       <c r="G66" s="45">
         <v>5.3174020769620602</v>
       </c>
@@ -12723,7 +12761,7 @@
       <c r="E67" s="44" t="s">
         <v>408</v>
       </c>
-      <c r="F67" s="44"/>
+      <c r="F67" s="99"/>
       <c r="G67" s="45">
         <v>8.4</v>
       </c>
@@ -12774,7 +12812,7 @@
       <c r="E68" s="44" t="s">
         <v>408</v>
       </c>
-      <c r="F68" s="44"/>
+      <c r="F68" s="99"/>
       <c r="G68" s="45">
         <v>0.8</v>
       </c>
@@ -12831,7 +12869,7 @@
       <c r="E69" s="44" t="s">
         <v>408</v>
       </c>
-      <c r="F69" s="44"/>
+      <c r="F69" s="100"/>
       <c r="G69" s="45">
         <v>3.2</v>
       </c>
@@ -12882,7 +12920,7 @@
       <c r="E70" s="44" t="s">
         <v>408</v>
       </c>
-      <c r="F70" s="44"/>
+      <c r="F70" s="100"/>
       <c r="G70" s="45">
         <v>32.5</v>
       </c>
@@ -12925,7 +12963,7 @@
       <c r="C71" s="43"/>
       <c r="D71" s="43"/>
       <c r="E71" s="44"/>
-      <c r="F71" s="44"/>
+      <c r="F71" s="99"/>
       <c r="G71" s="45"/>
       <c r="H71" s="46"/>
       <c r="I71" s="43"/>
@@ -12952,7 +12990,7 @@
       <c r="C72" s="43"/>
       <c r="D72" s="43"/>
       <c r="E72" s="44"/>
-      <c r="F72" s="44"/>
+      <c r="F72" s="100"/>
       <c r="G72" s="45"/>
       <c r="H72" s="46"/>
       <c r="I72" s="43"/>
@@ -12983,7 +13021,7 @@
       <c r="E73" s="44" t="s">
         <v>408</v>
       </c>
-      <c r="F73" s="44"/>
+      <c r="F73" s="100"/>
       <c r="G73" s="45">
         <v>4.5</v>
       </c>
@@ -13026,7 +13064,7 @@
       <c r="C74" s="43"/>
       <c r="D74" s="43"/>
       <c r="E74" s="44"/>
-      <c r="F74" s="44"/>
+      <c r="F74" s="100"/>
       <c r="G74" s="45"/>
       <c r="H74" s="46"/>
       <c r="I74" s="43"/>
@@ -13061,7 +13099,7 @@
       <c r="E75" s="44" t="s">
         <v>408</v>
       </c>
-      <c r="F75" s="44"/>
+      <c r="F75" s="100"/>
       <c r="G75" s="45">
         <v>28.1</v>
       </c>
@@ -13112,7 +13150,7 @@
       <c r="E76" s="44" t="s">
         <v>408</v>
       </c>
-      <c r="F76" s="44"/>
+      <c r="F76" s="100"/>
       <c r="G76" s="45">
         <v>16.5611787727746</v>
       </c>
@@ -13169,7 +13207,7 @@
       <c r="E77" s="44" t="s">
         <v>408</v>
       </c>
-      <c r="F77" s="44"/>
+      <c r="F77" s="100"/>
       <c r="G77" s="45">
         <v>9.9</v>
       </c>
@@ -13220,7 +13258,7 @@
       <c r="E78" s="44" t="s">
         <v>408</v>
       </c>
-      <c r="F78" s="44"/>
+      <c r="F78" s="100"/>
       <c r="G78" s="45">
         <v>22.1</v>
       </c>
@@ -13277,7 +13315,7 @@
       <c r="E79" s="44" t="s">
         <v>408</v>
       </c>
-      <c r="F79" s="44"/>
+      <c r="F79" s="100"/>
       <c r="G79" s="45">
         <v>20.6</v>
       </c>
@@ -13328,7 +13366,7 @@
       <c r="E80" s="44" t="s">
         <v>408</v>
       </c>
-      <c r="F80" s="44"/>
+      <c r="F80" s="100"/>
       <c r="G80" s="45">
         <v>3.9</v>
       </c>
@@ -13379,7 +13417,7 @@
       <c r="E81" s="44" t="s">
         <v>408</v>
       </c>
-      <c r="F81" s="44"/>
+      <c r="F81" s="100"/>
       <c r="G81" s="45">
         <v>46.4</v>
       </c>
@@ -13436,7 +13474,7 @@
       <c r="E82" s="44" t="s">
         <v>408</v>
       </c>
-      <c r="F82" s="44"/>
+      <c r="F82" s="99"/>
       <c r="G82" s="45">
         <v>18.2</v>
       </c>
@@ -13479,7 +13517,7 @@
       <c r="C83" s="43"/>
       <c r="D83" s="43"/>
       <c r="E83" s="44"/>
-      <c r="F83" s="44"/>
+      <c r="F83" s="100"/>
       <c r="G83" s="45"/>
       <c r="H83" s="46"/>
       <c r="I83" s="43"/>
@@ -13514,7 +13552,7 @@
       <c r="E84" s="44" t="s">
         <v>408</v>
       </c>
-      <c r="F84" s="44"/>
+      <c r="F84" s="100"/>
       <c r="G84" s="45">
         <v>24.277330890970319</v>
       </c>
@@ -13571,7 +13609,7 @@
       <c r="E85" s="44" t="s">
         <v>408</v>
       </c>
-      <c r="F85" s="44"/>
+      <c r="F85" s="100"/>
       <c r="G85" s="45">
         <v>13.759156663174062</v>
       </c>
@@ -13628,7 +13666,7 @@
       <c r="E86" s="44" t="s">
         <v>408</v>
       </c>
-      <c r="F86" s="44"/>
+      <c r="F86" s="99"/>
       <c r="G86" s="45">
         <v>12.9</v>
       </c>
@@ -13669,7 +13707,7 @@
       <c r="C87" s="43"/>
       <c r="D87" s="43"/>
       <c r="E87" s="44"/>
-      <c r="F87" s="44"/>
+      <c r="F87" s="100"/>
       <c r="G87" s="45"/>
       <c r="H87" s="46"/>
       <c r="I87" s="43"/>
@@ -13704,7 +13742,7 @@
       <c r="E88" s="44" t="s">
         <v>436</v>
       </c>
-      <c r="F88" s="44"/>
+      <c r="F88" s="100"/>
       <c r="G88" s="45">
         <v>4.5</v>
       </c>
@@ -13755,7 +13793,7 @@
       <c r="E89" s="44" t="s">
         <v>408</v>
       </c>
-      <c r="F89" s="44"/>
+      <c r="F89" s="100"/>
       <c r="G89" s="45">
         <v>22.5</v>
       </c>
@@ -13798,7 +13836,7 @@
       <c r="C90" s="43"/>
       <c r="D90" s="43"/>
       <c r="E90" s="44"/>
-      <c r="F90" s="44"/>
+      <c r="F90" s="100"/>
       <c r="G90" s="45"/>
       <c r="H90" s="46"/>
       <c r="I90" s="43"/>
@@ -13833,7 +13871,7 @@
       <c r="E91" s="44" t="s">
         <v>408</v>
       </c>
-      <c r="F91" s="44"/>
+      <c r="F91" s="100"/>
       <c r="G91" s="45">
         <v>33.669431027576444</v>
       </c>
@@ -13890,7 +13928,7 @@
       <c r="E92" s="44" t="s">
         <v>408</v>
       </c>
-      <c r="F92" s="44"/>
+      <c r="F92" s="100"/>
       <c r="G92" s="45">
         <v>8.4</v>
       </c>
@@ -13947,7 +13985,7 @@
       <c r="E93" s="44" t="s">
         <v>408</v>
       </c>
-      <c r="F93" s="44"/>
+      <c r="F93" s="100"/>
       <c r="G93" s="45">
         <v>47.77</v>
       </c>
@@ -14004,7 +14042,7 @@
       <c r="E94" s="44" t="s">
         <v>408</v>
       </c>
-      <c r="F94" s="44"/>
+      <c r="F94" s="100"/>
       <c r="G94" s="45">
         <v>31.1</v>
       </c>
@@ -14047,7 +14085,7 @@
       <c r="C95" s="43"/>
       <c r="D95" s="43"/>
       <c r="E95" s="44"/>
-      <c r="F95" s="44"/>
+      <c r="F95" s="100"/>
       <c r="G95" s="45"/>
       <c r="H95" s="46"/>
       <c r="I95" s="43"/>
@@ -14074,7 +14112,7 @@
       <c r="C96" s="43"/>
       <c r="D96" s="43"/>
       <c r="E96" s="44"/>
-      <c r="F96" s="44"/>
+      <c r="F96" s="100"/>
       <c r="G96" s="45"/>
       <c r="H96" s="46"/>
       <c r="I96" s="43"/>
@@ -14097,7 +14135,7 @@
       <c r="C97" s="43"/>
       <c r="D97" s="43"/>
       <c r="E97" s="44"/>
-      <c r="F97" s="44"/>
+      <c r="F97" s="100"/>
       <c r="G97" s="45"/>
       <c r="H97" s="46"/>
       <c r="I97" s="43"/>
@@ -14132,7 +14170,7 @@
       <c r="E98" s="44" t="s">
         <v>436</v>
       </c>
-      <c r="F98" s="44"/>
+      <c r="F98" s="99"/>
       <c r="G98" s="45">
         <v>12.998149731841657</v>
       </c>
@@ -14189,7 +14227,7 @@
       <c r="E99" s="44" t="s">
         <v>408</v>
       </c>
-      <c r="F99" s="44"/>
+      <c r="F99" s="99"/>
       <c r="G99" s="45">
         <v>4.4680961914898374</v>
       </c>
@@ -14238,7 +14276,7 @@
       <c r="C100" s="43"/>
       <c r="D100" s="43"/>
       <c r="E100" s="44"/>
-      <c r="F100" s="44"/>
+      <c r="F100" s="100"/>
       <c r="G100" s="45"/>
       <c r="H100" s="46"/>
       <c r="I100" s="43"/>
@@ -14269,7 +14307,7 @@
       <c r="E101" s="44" t="s">
         <v>436</v>
       </c>
-      <c r="F101" s="44"/>
+      <c r="F101" s="100"/>
       <c r="G101" s="45">
         <v>15.3</v>
       </c>
@@ -14326,7 +14364,7 @@
       <c r="E102" s="44" t="s">
         <v>417</v>
       </c>
-      <c r="F102" s="44"/>
+      <c r="F102" s="100"/>
       <c r="G102" s="45">
         <v>19.383336322914499</v>
       </c>
@@ -14377,7 +14415,7 @@
       <c r="E103" s="44" t="s">
         <v>408</v>
       </c>
-      <c r="F103" s="44"/>
+      <c r="F103" s="100"/>
       <c r="G103" s="45">
         <v>11</v>
       </c>
@@ -14426,7 +14464,7 @@
       <c r="C104" s="43"/>
       <c r="D104" s="43"/>
       <c r="E104" s="44"/>
-      <c r="F104" s="44"/>
+      <c r="F104" s="100"/>
       <c r="G104" s="45"/>
       <c r="H104" s="46"/>
       <c r="I104" s="45"/>
@@ -14449,7 +14487,7 @@
       <c r="C105" s="43"/>
       <c r="D105" s="43"/>
       <c r="E105" s="44"/>
-      <c r="F105" s="44"/>
+      <c r="F105" s="99"/>
       <c r="G105" s="45"/>
       <c r="H105" s="46"/>
       <c r="I105" s="43"/>
@@ -14484,7 +14522,7 @@
       <c r="E106" s="44" t="s">
         <v>408</v>
       </c>
-      <c r="F106" s="44"/>
+      <c r="F106" s="100"/>
       <c r="G106" s="45">
         <v>16.100000000000001</v>
       </c>
@@ -14527,7 +14565,7 @@
       <c r="C107" s="58"/>
       <c r="D107" s="58"/>
       <c r="E107" s="59"/>
-      <c r="F107" s="59"/>
+      <c r="F107" s="100"/>
       <c r="G107" s="60"/>
       <c r="H107" s="61"/>
       <c r="I107" s="58"/>
@@ -14550,7 +14588,7 @@
       <c r="C108" s="58"/>
       <c r="D108" s="58"/>
       <c r="E108" s="59"/>
-      <c r="F108" s="59"/>
+      <c r="F108" s="100"/>
       <c r="G108" s="60"/>
       <c r="H108" s="61"/>
       <c r="I108" s="58"/>
@@ -14577,7 +14615,7 @@
       <c r="C109" s="58"/>
       <c r="D109" s="58"/>
       <c r="E109" s="59"/>
-      <c r="F109" s="59"/>
+      <c r="F109" s="99"/>
       <c r="G109" s="60"/>
       <c r="H109" s="61"/>
       <c r="I109" s="58"/>
@@ -14604,7 +14642,7 @@
       <c r="C110" s="58"/>
       <c r="D110" s="58"/>
       <c r="E110" s="59"/>
-      <c r="F110" s="59"/>
+      <c r="F110" s="100"/>
       <c r="G110" s="60"/>
       <c r="H110" s="61"/>
       <c r="I110" s="58"/>
@@ -14631,7 +14669,7 @@
       <c r="C111" s="43"/>
       <c r="D111" s="43"/>
       <c r="E111" s="44"/>
-      <c r="F111" s="44"/>
+      <c r="F111" s="100"/>
       <c r="G111" s="45"/>
       <c r="H111" s="46"/>
       <c r="I111" s="43"/>
@@ -14666,7 +14704,7 @@
       <c r="E112" s="44" t="s">
         <v>408</v>
       </c>
-      <c r="F112" s="44"/>
+      <c r="F112" s="100"/>
       <c r="G112" s="45">
         <v>15.4</v>
       </c>
@@ -14717,7 +14755,7 @@
       <c r="E113" s="64" t="s">
         <v>408</v>
       </c>
-      <c r="F113" s="64"/>
+      <c r="F113" s="100"/>
       <c r="G113" s="45">
         <v>14.9</v>
       </c>
@@ -14768,7 +14806,7 @@
       <c r="E114" s="44" t="s">
         <v>408</v>
       </c>
-      <c r="F114" s="44"/>
+      <c r="F114" s="100"/>
       <c r="G114" s="45">
         <v>6</v>
       </c>
@@ -14809,7 +14847,7 @@
       <c r="C115" s="58"/>
       <c r="D115" s="58"/>
       <c r="E115" s="59"/>
-      <c r="F115" s="59"/>
+      <c r="F115" s="100"/>
       <c r="G115" s="60"/>
       <c r="H115" s="61"/>
       <c r="I115" s="58"/>
@@ -14844,7 +14882,7 @@
       <c r="E116" s="53" t="s">
         <v>408</v>
       </c>
-      <c r="F116" s="53"/>
+      <c r="F116" s="99"/>
       <c r="G116" s="54">
         <v>34.700000000000003</v>
       </c>
@@ -14887,7 +14925,7 @@
       <c r="C117" s="58"/>
       <c r="D117" s="58"/>
       <c r="E117" s="59"/>
-      <c r="F117" s="59"/>
+      <c r="F117" s="100"/>
       <c r="G117" s="60"/>
       <c r="H117" s="61"/>
       <c r="I117" s="58"/>
@@ -14922,7 +14960,7 @@
       <c r="E118" s="44" t="s">
         <v>408</v>
       </c>
-      <c r="F118" s="44"/>
+      <c r="F118" s="100"/>
       <c r="G118" s="45">
         <v>39.799999999999997</v>
       </c>
@@ -14961,7 +14999,7 @@
       <c r="C119" s="58"/>
       <c r="D119" s="58"/>
       <c r="E119" s="59"/>
-      <c r="F119" s="59"/>
+      <c r="F119" s="99"/>
       <c r="G119" s="60"/>
       <c r="H119" s="61"/>
       <c r="I119" s="58"/>
@@ -14996,7 +15034,7 @@
       <c r="E120" s="44" t="s">
         <v>436</v>
       </c>
-      <c r="F120" s="44"/>
+      <c r="F120" s="100"/>
       <c r="G120" s="45">
         <v>45.6</v>
       </c>
@@ -15049,7 +15087,7 @@
       <c r="E121" s="59" t="s">
         <v>408</v>
       </c>
-      <c r="F121" s="59"/>
+      <c r="F121" s="100"/>
       <c r="G121" s="60">
         <v>9.17</v>
       </c>
@@ -15106,7 +15144,7 @@
       <c r="E122" s="44" t="s">
         <v>408</v>
       </c>
-      <c r="F122" s="44"/>
+      <c r="F122" s="100"/>
       <c r="G122" s="45">
         <v>6.445392531366319</v>
       </c>
@@ -15157,7 +15195,7 @@
       <c r="E123" s="44" t="s">
         <v>408</v>
       </c>
-      <c r="F123" s="44"/>
+      <c r="F123" s="100"/>
       <c r="G123" s="45">
         <v>11.729758575995989</v>
       </c>
@@ -15208,7 +15246,7 @@
       <c r="E124" s="53" t="s">
         <v>408</v>
       </c>
-      <c r="F124" s="53"/>
+      <c r="F124" s="100"/>
       <c r="G124" s="54">
         <v>25.1</v>
       </c>
@@ -15259,7 +15297,7 @@
       <c r="E125" s="53" t="s">
         <v>408</v>
       </c>
-      <c r="F125" s="53"/>
+      <c r="F125" s="99"/>
       <c r="G125" s="54">
         <v>13</v>
       </c>
@@ -15306,7 +15344,7 @@
       <c r="E126" s="44" t="s">
         <v>436</v>
       </c>
-      <c r="F126" s="44"/>
+      <c r="F126" s="100"/>
       <c r="G126" s="45">
         <v>19.899999999999999</v>
       </c>
@@ -15363,7 +15401,7 @@
       <c r="E127" s="53" t="s">
         <v>408</v>
       </c>
-      <c r="F127" s="53"/>
+      <c r="F127" s="100"/>
       <c r="G127" s="54">
         <v>35.700000000000003</v>
       </c>
@@ -15406,7 +15444,7 @@
       <c r="C128" s="58"/>
       <c r="D128" s="58"/>
       <c r="E128" s="59"/>
-      <c r="F128" s="59"/>
+      <c r="F128" s="100"/>
       <c r="G128" s="60"/>
       <c r="H128" s="61"/>
       <c r="I128" s="58"/>
@@ -15429,7 +15467,7 @@
       <c r="C129" s="58"/>
       <c r="D129" s="58"/>
       <c r="E129" s="59"/>
-      <c r="F129" s="59"/>
+      <c r="F129" s="100"/>
       <c r="G129" s="60"/>
       <c r="H129" s="61"/>
       <c r="I129" s="58"/>
@@ -15464,7 +15502,7 @@
       <c r="E130" s="44" t="s">
         <v>408</v>
       </c>
-      <c r="F130" s="44"/>
+      <c r="F130" s="100"/>
       <c r="G130" s="45">
         <v>3</v>
       </c>
@@ -15507,7 +15545,7 @@
       <c r="C131" s="43"/>
       <c r="D131" s="43"/>
       <c r="E131" s="44"/>
-      <c r="F131" s="44"/>
+      <c r="F131" s="100"/>
       <c r="G131" s="45"/>
       <c r="H131" s="46"/>
       <c r="I131" s="43"/>
@@ -15542,7 +15580,7 @@
       <c r="E132" s="44" t="s">
         <v>417</v>
       </c>
-      <c r="F132" s="44"/>
+      <c r="F132" s="100"/>
       <c r="G132" s="45">
         <v>2.6</v>
       </c>
@@ -15591,7 +15629,7 @@
       <c r="C133" s="43"/>
       <c r="D133" s="43"/>
       <c r="E133" s="44"/>
-      <c r="F133" s="44"/>
+      <c r="F133" s="100"/>
       <c r="G133" s="45"/>
       <c r="H133" s="46"/>
       <c r="I133" s="43"/>
@@ -15618,7 +15656,7 @@
       <c r="C134" s="43"/>
       <c r="D134" s="43"/>
       <c r="E134" s="44"/>
-      <c r="F134" s="44"/>
+      <c r="F134" s="100"/>
       <c r="G134" s="45"/>
       <c r="H134" s="46"/>
       <c r="I134" s="43"/>
@@ -15653,7 +15691,7 @@
       <c r="E135" s="44" t="s">
         <v>408</v>
       </c>
-      <c r="F135" s="44"/>
+      <c r="F135" s="100"/>
       <c r="G135" s="45">
         <v>30.9</v>
       </c>
@@ -15710,7 +15748,7 @@
       <c r="E136" s="44" t="s">
         <v>408</v>
       </c>
-      <c r="F136" s="44"/>
+      <c r="F136" s="100"/>
       <c r="G136" s="45">
         <v>15.1</v>
       </c>
@@ -15761,7 +15799,7 @@
       <c r="E137" s="44" t="s">
         <v>408</v>
       </c>
-      <c r="F137" s="44"/>
+      <c r="F137" s="100"/>
       <c r="G137" s="45">
         <v>6.1</v>
       </c>
@@ -15818,7 +15856,7 @@
       <c r="E138" s="44" t="s">
         <v>408</v>
       </c>
-      <c r="F138" s="44"/>
+      <c r="F138" s="100"/>
       <c r="G138" s="45">
         <v>4.3</v>
       </c>
@@ -15861,7 +15899,7 @@
       <c r="C139" s="58"/>
       <c r="D139" s="58"/>
       <c r="E139" s="59"/>
-      <c r="F139" s="59"/>
+      <c r="F139" s="99"/>
       <c r="G139" s="60"/>
       <c r="H139" s="61"/>
       <c r="I139" s="58"/>
@@ -15896,7 +15934,7 @@
       <c r="E140" s="43" t="s">
         <v>436</v>
       </c>
-      <c r="F140" s="43"/>
+      <c r="F140" s="100"/>
       <c r="G140" s="43">
         <v>5.0999999999999996</v>
       </c>
@@ -15945,7 +15983,7 @@
       <c r="C141" s="43"/>
       <c r="D141" s="43"/>
       <c r="E141" s="43"/>
-      <c r="F141" s="43"/>
+      <c r="F141" s="100"/>
       <c r="G141" s="43"/>
       <c r="H141" s="46"/>
       <c r="I141" s="45"/>
@@ -15968,7 +16006,7 @@
       <c r="C142" s="43"/>
       <c r="D142" s="43"/>
       <c r="E142" s="43"/>
-      <c r="F142" s="43"/>
+      <c r="F142" s="100"/>
       <c r="G142" s="43"/>
       <c r="H142" s="46"/>
       <c r="I142" s="45"/>
@@ -15995,7 +16033,7 @@
       <c r="C143" s="43"/>
       <c r="D143" s="43"/>
       <c r="E143" s="43"/>
-      <c r="F143" s="43"/>
+      <c r="F143" s="100"/>
       <c r="G143" s="43"/>
       <c r="H143" s="46"/>
       <c r="I143" s="45"/>
@@ -16026,7 +16064,7 @@
       <c r="E144" s="44" t="s">
         <v>408</v>
       </c>
-      <c r="F144" s="44"/>
+      <c r="F144" s="99"/>
       <c r="G144" s="45">
         <v>13.569449365627856</v>
       </c>
@@ -16083,7 +16121,7 @@
       <c r="E145" s="44" t="s">
         <v>408</v>
       </c>
-      <c r="F145" s="44"/>
+      <c r="F145" s="100"/>
       <c r="G145" s="45">
         <v>28.1</v>
       </c>
@@ -16132,7 +16170,7 @@
       <c r="C146" s="58"/>
       <c r="D146" s="58"/>
       <c r="E146" s="59"/>
-      <c r="F146" s="59"/>
+      <c r="F146" s="100"/>
       <c r="G146" s="60"/>
       <c r="H146" s="61"/>
       <c r="I146" s="58"/>
@@ -16148,34 +16186,42 @@
       <c r="S146" s="45"/>
     </row>
     <row r="147" spans="1:19">
+      <c r="F147" s="100"/>
       <c r="R147" s="76"/>
       <c r="S147" s="76"/>
     </row>
     <row r="148" spans="1:19">
+      <c r="F148" s="100"/>
       <c r="R148" s="76"/>
       <c r="S148" s="76"/>
     </row>
     <row r="149" spans="1:19">
+      <c r="F149" s="99"/>
       <c r="R149" s="76"/>
       <c r="S149" s="76"/>
     </row>
     <row r="150" spans="1:19">
+      <c r="F150" s="100"/>
       <c r="R150" s="76"/>
       <c r="S150" s="76"/>
     </row>
     <row r="151" spans="1:19">
+      <c r="F151" s="100"/>
       <c r="R151" s="76"/>
       <c r="S151" s="76"/>
     </row>
     <row r="152" spans="1:19">
+      <c r="F152" s="100"/>
       <c r="R152" s="76"/>
       <c r="S152" s="76"/>
     </row>
     <row r="153" spans="1:19">
+      <c r="F153" s="100"/>
       <c r="R153" s="76"/>
       <c r="S153" s="76"/>
     </row>
     <row r="154" spans="1:19">
+      <c r="F154" s="100"/>
       <c r="R154" s="76"/>
       <c r="S154" s="76"/>
     </row>

</xml_diff>